<commit_message>
Add possibility to upload xls files
</commit_message>
<xml_diff>
--- a/taps.xlsx
+++ b/taps.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="4860" yWindow="1380" windowWidth="19140" windowHeight="12280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="42">
   <si>
     <t>XPA</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Guenrouët, Loire-Atlantique France</t>
   </si>
   <si>
-    <t>Kriek</t>
-  </si>
-  <si>
     <t>5.5%</t>
   </si>
   <si>
@@ -102,9 +99,6 @@
     <t>8.0%</t>
   </si>
   <si>
-    <t>3.5%</t>
-  </si>
-  <si>
     <t>tapNumber</t>
   </si>
   <si>
@@ -133,13 +127,31 @@
   </si>
   <si>
     <t>price050</t>
+  </si>
+  <si>
+    <t>Слёзы Фрейи</t>
+  </si>
+  <si>
+    <t>IsKra Brewery</t>
+  </si>
+  <si>
+    <t>Scandinavian Pale Ale</t>
+  </si>
+  <si>
+    <t>Hasta Mañana, Amigos!</t>
+  </si>
+  <si>
+    <t>Bottle Share (Планета Земля)</t>
+  </si>
+  <si>
+    <t>Gose</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -171,6 +183,12 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -189,7 +207,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -219,12 +237,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="29"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="30">
+    <cellStyle name="Excel Built-in Normal" xfId="29"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -585,7 +607,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B9" sqref="B9:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -600,34 +622,34 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>33</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>34</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>35</v>
-      </c>
-      <c r="I1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -647,7 +669,7 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H2">
         <v>180</v>
@@ -676,7 +698,7 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H3">
         <v>170</v>
@@ -702,7 +724,7 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4">
         <v>200</v>
@@ -731,7 +753,7 @@
         <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H5">
         <v>300</v>
@@ -760,7 +782,7 @@
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6">
         <v>100</v>
@@ -789,7 +811,7 @@
         <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H7">
         <v>200</v>
@@ -815,7 +837,7 @@
         <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H8">
         <v>230</v>
@@ -825,26 +847,28 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9">
+      <c r="B9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="2">
+        <v>15</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2">
         <v>200</v>
       </c>
-      <c r="I9">
-        <v>340</v>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2">
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -864,7 +888,7 @@
         <v>3</v>
       </c>
       <c r="F10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H10">
         <v>230</v>
@@ -887,7 +911,7 @@
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G11">
         <v>100</v>
@@ -916,7 +940,7 @@
         <v>3</v>
       </c>
       <c r="F12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H12">
         <v>200</v>
@@ -932,26 +956,28 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13">
-        <v>200</v>
-      </c>
-      <c r="I13">
-        <v>340</v>
+      <c r="B13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="2">
+        <v>40</v>
+      </c>
+      <c r="F13" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2">
+        <v>220</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2">
+        <v>250</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -971,7 +997,7 @@
         <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H14">
         <v>200</v>
@@ -997,7 +1023,7 @@
         <v>3</v>
       </c>
       <c r="F15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H15">
         <v>170</v>
@@ -1023,7 +1049,7 @@
         <v>41</v>
       </c>
       <c r="F16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H16">
         <v>300</v>
@@ -1052,7 +1078,7 @@
         <v>3</v>
       </c>
       <c r="F17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H17">
         <v>180</v>
@@ -1072,7 +1098,6 @@
     <sortCondition ref="B10"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>